<commit_message>
Estou enviando a tabela bonita, mas pode pegar o SQL
</commit_message>
<xml_diff>
--- a/2ª Etapa do Projeto - Modelo Lógico/Template Table Logical Dictionary/Template Table Logical Dictionary.xlsx
+++ b/2ª Etapa do Projeto - Modelo Lógico/Template Table Logical Dictionary/Template Table Logical Dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nena\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nena\Desktop\Rômulo\SisGAF\SisGAF\2ª Etapa do Projeto - Modelo Lógico\Template Table Logical Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Atributo</t>
   </si>
@@ -41,26 +41,29 @@
     <t/>
   </si>
   <si>
-    <t>x</t>
+    <t>Domínio</t>
   </si>
   <si>
-    <t>&lt;ENTIDADE&gt;: &lt;Descrição&gt;</t>
-  </si>
-  <si>
-    <t>Repetições</t>
-  </si>
-  <si>
-    <t>Usado para guardar o número de repetições do cliente</t>
-  </si>
-  <si>
-    <t>Series</t>
+    <r>
+      <t xml:space="preserve">&lt;ENTIDADE&gt;: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;Descrição&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +81,13 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -111,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -225,13 +235,33 @@
       <bottom style="thin">
         <color theme="1" tint="0.499984740745262"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -249,16 +279,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -277,6 +301,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,248 +592,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="5" width="21.42578125" customWidth="1"/>
+    <col min="2" max="6" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="7" t="s">
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="11" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="14"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="5"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="5"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>